<commit_message>
done placeOrder, addMedia and payOrder
</commit_message>
<xml_diff>
--- a/lab02-AddMediaToCart/placeOrder.xlsx
+++ b/lab02-AddMediaToCart/placeOrder.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23318"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUST\Desktop\Software Development\lab02-AddMediaToCart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8044FE34-AA92-4A2F-9CAF-34A6AD4B3F2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C728E2AE-7E60-4F11-BACC-B27ACDC1843C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A5862D3A-5575-4B60-A058-3FEBD154D1E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,24 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
-  <si>
-    <t>place order</t>
-  </si>
-  <si>
-    <t>pay order</t>
-  </si>
-  <si>
-    <t>add media</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specification </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tabular </t>
-  </si>
-  <si>
-    <t>activity diagram</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+  <si>
+    <t>USE CASE</t>
+  </si>
+  <si>
+    <t>ADD MEDIA TO CART</t>
   </si>
   <si>
     <t>Success/Basic flow</t>
@@ -104,22 +93,70 @@
     <t>the use case ends</t>
   </si>
   <si>
-    <t>USE CASE</t>
-  </si>
-  <si>
-    <t>ADD MEDIA TO CART</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLACE ORDER </t>
+    <t>PLACE ORDER</t>
   </si>
   <si>
     <t>send requests to place order</t>
   </si>
   <si>
-    <t>check if cart is not empty and all media are available</t>
+    <t>check if all media are available</t>
+  </si>
+  <si>
+    <t>prompt detail information screen for placing order</t>
   </si>
   <si>
     <t>enter detail information for shipping and choose shipping method</t>
+  </si>
+  <si>
+    <t>check if address is available to delivery</t>
+  </si>
+  <si>
+    <t>calculate total amount of money customer has to pay, includes shipping fee and display for customer</t>
+  </si>
+  <si>
+    <t>submit request to place order</t>
+  </si>
+  <si>
+    <t>calls use case "Pay order"</t>
+  </si>
+  <si>
+    <t>notifies that placing order is successful</t>
+  </si>
+  <si>
+    <t>at any time</t>
+  </si>
+  <si>
+    <t>cancels placing order at anytime</t>
+  </si>
+  <si>
+    <t>notifies that some items are not available right now</t>
+  </si>
+  <si>
+    <t>Step 5 of Basic flow</t>
+  </si>
+  <si>
+    <t>notifies that customer's address is not available to delivery</t>
+  </si>
+  <si>
+    <t>back to Step 4 of Basic flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAY ORDER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">send requests with customer's card and amount of money to pay order </t>
+  </si>
+  <si>
+    <t>Interbank</t>
+  </si>
+  <si>
+    <t>check if balance of card is enough for purchasing</t>
+  </si>
+  <si>
+    <t>send response to Software that transaction is successful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notifies that balance is not enough for purchasing </t>
   </si>
 </sst>
 </file>
@@ -127,9 +164,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +199,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -177,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -185,39 +231,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -534,301 +595,440 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E365C12-B0A5-4D97-88B8-454CFC6625E3}">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G24" sqref="F24:G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="3" spans="1:4" ht="29.25" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="37.5" customHeight="1">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="26.25" customHeight="1">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27" customHeight="1">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.25" customHeight="1">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" ht="12" customHeight="1"/>
+    <row r="11" spans="1:4" ht="21" customHeight="1">
+      <c r="A11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="11"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="41.25" customHeight="1">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="17" spans="1:4" ht="37.5" customHeight="1">
+      <c r="A17" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="45">
+      <c r="A19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30">
+      <c r="A23" s="2">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30">
+      <c r="A24" s="2">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="9" t="s">
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2">
+        <v>5</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T2" s="1" t="s">
+    <row r="26" spans="1:4" ht="45">
+      <c r="A26" s="2">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2">
+        <v>8</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2">
+        <v>9</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="32" spans="1:4" ht="30" customHeight="1">
+      <c r="A32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30">
+      <c r="A35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30">
+      <c r="A36" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+    </row>
+    <row r="41" spans="1:4" ht="37.5" customHeight="1">
+      <c r="A41" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="43" spans="1:4" ht="45" customHeight="1">
+      <c r="A43" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="T3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="T4" s="1" t="s">
+      <c r="B43" s="11"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="30">
+      <c r="A45" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="B45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30">
+      <c r="A46" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="30">
+      <c r="A47" s="2">
+        <v>3</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1">
+      <c r="A50" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="B50" s="11"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B51" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="T7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="C51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="T8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="52" spans="1:4" ht="30">
+      <c r="A52" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="B52" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>1</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>2</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>3</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A41:B41"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>